<commit_message>
major updates detaching taxonomic information from folders; logging system added; folders reorganized
</commit_message>
<xml_diff>
--- a/SPPDATA_EX.xlsx
+++ b/SPPDATA_EX.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Garcilazo\Javascript_NodeJS\FAPOWebpage\02_Editing_Dynamic\PYTHON_Version\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8559A360-DD8E-413C-A833-BE356CAE8426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPECIES DATA" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -83,9 +93,6 @@
     <t>Salgueiro-Sepúlveda</t>
   </si>
   <si>
-    <t>SYMPHY0143</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidersp:009027]</t>
   </si>
   <si>
@@ -107,9 +114,6 @@
     <t>Epilineutes sp01</t>
   </si>
   <si>
-    <t>THERSM0212</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidergen:00739]</t>
   </si>
   <si>
@@ -122,9 +126,6 @@
     <t>Epilineutes sp02</t>
   </si>
   <si>
-    <t>THERSM0213</t>
-  </si>
-  <si>
     <t>TXV085</t>
   </si>
   <si>
@@ -134,9 +135,6 @@
     <t>Chthonos sp01</t>
   </si>
   <si>
-    <t>THERID0190</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidergen:00737]</t>
   </si>
   <si>
@@ -155,9 +153,6 @@
     <t>Theridiosoma chiripa</t>
   </si>
   <si>
-    <t>THERSM0214</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidersp:039839]</t>
   </si>
   <si>
@@ -173,9 +168,6 @@
     <t>Theridiosoma sp01</t>
   </si>
   <si>
-    <t>THERSM0215</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidergen:00744]</t>
   </si>
   <si>
@@ -186,13 +178,31 @@
   </si>
   <si>
     <t>Phoroncidia sp01</t>
+  </si>
+  <si>
+    <t>INVTUXV212</t>
+  </si>
+  <si>
+    <t>INVTUXV213</t>
+  </si>
+  <si>
+    <t>INVTUXV214</t>
+  </si>
+  <si>
+    <t>INVTUXV216</t>
+  </si>
+  <si>
+    <t>INVTUXV217</t>
+  </si>
+  <si>
+    <t>INVTUXV215</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,13 +256,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,9 +356,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,6 +408,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -554,30 +601,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.26171875" customWidth="1"/>
+    <col min="5" max="5" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75">
+    <row r="1" spans="1:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -624,7 +671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -634,23 +681,23 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -669,21 +716,21 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -692,10 +739,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -714,21 +761,21 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -737,10 +784,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -759,21 +806,21 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -782,13 +829,13 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -797,40 +844,40 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" t="s">
-        <v>48</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -849,21 +896,21 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -872,10 +919,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -894,620 +941,620 @@
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4"/>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4"/>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4"/>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4"/>
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4"/>
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4"/>
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4"/>
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4"/>
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4"/>
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4"/>
       <c r="P53" s="4"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4"/>
       <c r="P54" s="4"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
       <c r="P55" s="4"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4"/>
       <c r="P56" s="4"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3"/>
       <c r="P57" s="4"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4"/>
       <c r="P58" s="3"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4"/>
       <c r="P60" s="4"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4"/>
       <c r="P61" s="4"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="4"/>
       <c r="P62" s="4"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="4"/>
       <c r="P63" s="4"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="4"/>
       <c r="P64" s="4"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="4"/>
       <c r="P65" s="4"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="4"/>
       <c r="P66" s="4"/>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="4"/>
       <c r="P67" s="4"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="4"/>
       <c r="P68" s="4"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4"/>
       <c r="P69" s="4"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4"/>
       <c r="P70" s="4"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4"/>
       <c r="P71" s="4"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="4"/>
       <c r="P72" s="4"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4"/>
       <c r="P73" s="4"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4"/>
       <c r="P74" s="4"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="4"/>
       <c r="P75" s="4"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="4"/>
       <c r="P76" s="4"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="4"/>
       <c r="P77" s="4"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="4"/>
       <c r="P78" s="4"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4"/>
       <c r="P79" s="4"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4"/>
       <c r="P80" s="4"/>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="4"/>
       <c r="P81" s="4"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="4"/>
       <c r="P82" s="4"/>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="4"/>
       <c r="P83" s="4"/>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4"/>
       <c r="P84" s="4"/>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4"/>
       <c r="P85" s="4"/>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4"/>
       <c r="P86" s="4"/>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4"/>
       <c r="P87" s="4"/>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4"/>
       <c r="P88" s="4"/>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4"/>
       <c r="P89" s="3"/>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="4"/>
       <c r="P90" s="4"/>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="4"/>
       <c r="P91" s="4"/>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4"/>
       <c r="P92" s="4"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="4"/>
       <c r="P93" s="4"/>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="4"/>
       <c r="P94" s="4"/>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4"/>
       <c r="P95" s="4"/>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4"/>
       <c r="P96" s="4"/>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="4"/>
       <c r="P97" s="4"/>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="4"/>
       <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="4"/>
       <c r="P99" s="4"/>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4"/>
       <c r="P100" s="4"/>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4"/>
       <c r="P101" s="4"/>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="4"/>
       <c r="P102" s="4"/>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4"/>
       <c r="P103" s="4"/>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="4"/>
       <c r="P104" s="4"/>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4"/>
       <c r="P105" s="4"/>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="4"/>
       <c r="P106" s="4"/>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4"/>
       <c r="P107" s="4"/>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4"/>
       <c r="P108" s="4"/>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="4"/>
       <c r="P109" s="4"/>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="4"/>
       <c r="P110" s="4"/>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4"/>
       <c r="P111" s="4"/>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="4"/>
       <c r="P112" s="4"/>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="4"/>
       <c r="P113" s="4"/>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="4"/>
       <c r="P114" s="4"/>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="4"/>
       <c r="P115" s="4"/>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="4"/>
       <c r="P116" s="4"/>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="4"/>
       <c r="P117" s="4"/>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="4"/>
       <c r="P118" s="4"/>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="4"/>
       <c r="P119" s="4"/>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="4"/>
       <c r="P120" s="4"/>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="4"/>
       <c r="P121" s="4"/>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="4"/>
       <c r="P122" s="4"/>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="4"/>
       <c r="P123" s="4"/>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="4"/>
       <c r="P124" s="4"/>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="4"/>
       <c r="P125" s="4"/>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="4"/>
       <c r="P126" s="4"/>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4"/>
       <c r="P127" s="4"/>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="4"/>
       <c r="P128" s="4"/>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="4"/>
       <c r="P129" s="4"/>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="4"/>
       <c r="P130" s="4"/>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="4"/>
       <c r="P131" s="4"/>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="4"/>
       <c r="P132" s="4"/>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="4"/>
       <c r="P133" s="4"/>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="4"/>
       <c r="P134" s="4"/>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="4"/>
       <c r="P135" s="4"/>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="4"/>
       <c r="P136" s="4"/>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="4"/>
       <c r="P137" s="4"/>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="4"/>
       <c r="P138" s="4"/>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="4"/>
       <c r="P139" s="4"/>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="4"/>
       <c r="P140" s="4"/>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="4"/>
       <c r="P141" s="4"/>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="4"/>
       <c r="P142" s="4"/>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="4"/>
       <c r="P143" s="4"/>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="P144" s="4"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="4"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="4"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="4"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="4"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="4"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="4"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="4"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="4"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="4"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="4"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="4"/>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="4"/>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="4"/>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="4"/>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="4"/>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="4"/>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="4"/>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="4"/>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="4"/>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="4"/>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="4"/>
     </row>
-    <row r="172" spans="1:13" ht="16.5">
+    <row r="172" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -1522,7 +1569,7 @@
       <c r="L172" s="5"/>
       <c r="M172" s="5"/>
     </row>
-    <row r="173" spans="1:13" ht="16.5">
+    <row r="173" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -1537,7 +1584,7 @@
       <c r="L173" s="5"/>
       <c r="M173" s="5"/>
     </row>
-    <row r="174" spans="1:13" ht="16.5">
+    <row r="174" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -1552,7 +1599,7 @@
       <c r="L174" s="5"/>
       <c r="M174" s="5"/>
     </row>
-    <row r="175" spans="1:13" ht="16.5">
+    <row r="175" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -1567,7 +1614,7 @@
       <c r="L175" s="5"/>
       <c r="M175" s="5"/>
     </row>
-    <row r="176" spans="1:13" ht="16.5">
+    <row r="176" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -1581,7 +1628,7 @@
       <c r="L176" s="5"/>
       <c r="M176" s="5"/>
     </row>
-    <row r="177" spans="1:13" ht="16.5">
+    <row r="177" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -1595,7 +1642,7 @@
       <c r="L177" s="5"/>
       <c r="M177" s="5"/>
     </row>
-    <row r="178" spans="1:13" ht="16.5">
+    <row r="178" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -1609,1203 +1656,1203 @@
       <c r="L178" s="5"/>
       <c r="M178" s="5"/>
     </row>
-    <row r="179" spans="1:13" ht="15.75">
+    <row r="179" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="1:13" ht="15.75">
+    <row r="180" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="1:13" ht="15.75">
+    <row r="181" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="1:13" ht="15.75">
+    <row r="182" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="1:13" ht="15.75">
+    <row r="183" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="1:13" ht="15.75">
+    <row r="184" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="1:13" ht="15.75">
+    <row r="185" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="1:13" ht="15.75">
+    <row r="186" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="1:13" ht="15.75">
+    <row r="187" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="1:13" ht="15.75">
+    <row r="188" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="1:13" ht="15.75">
+    <row r="189" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="1:13" ht="15.75">
+    <row r="190" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="1:13" ht="15.75">
+    <row r="191" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="1:13" ht="15.75">
+    <row r="192" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="2:4" ht="15.75">
+    <row r="193" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="2:4" ht="15.75">
+    <row r="194" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="2:4" ht="15.75">
+    <row r="195" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="2:4" ht="15.75">
+    <row r="196" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="2:4" ht="15.75">
+    <row r="197" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="2:4" ht="15.75">
+    <row r="198" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="2:4" ht="15.75">
+    <row r="199" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="2:4" ht="15.75">
+    <row r="200" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="2:4" ht="15.75">
+    <row r="201" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="2:4" ht="15.75">
+    <row r="202" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="2:4" ht="15.75">
+    <row r="203" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="2:4" ht="15.75">
+    <row r="204" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="2:4" ht="15.75">
+    <row r="205" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="2:4" ht="15.75">
+    <row r="206" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="2:4" ht="15.75">
+    <row r="207" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="2:4" ht="15.75">
+    <row r="208" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="2:16" ht="15.75">
+    <row r="209" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="2:16" ht="15.75">
+    <row r="210" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="2:16" ht="15.75">
+    <row r="211" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="2:16" ht="15.75">
+    <row r="212" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="P212" s="4"/>
     </row>
-    <row r="213" spans="2:16" ht="15.75">
+    <row r="213" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="P213" s="4"/>
     </row>
-    <row r="214" spans="2:16" ht="15.75">
+    <row r="214" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="P214" s="4"/>
     </row>
-    <row r="215" spans="2:16" ht="15.75">
+    <row r="215" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="P215" s="4"/>
     </row>
-    <row r="216" spans="2:16" ht="15.75">
+    <row r="216" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="P216" s="4"/>
     </row>
-    <row r="217" spans="2:16" ht="15.75">
+    <row r="217" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="P217" s="4"/>
     </row>
-    <row r="218" spans="2:16" ht="15.75">
+    <row r="218" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="P218" s="4"/>
     </row>
-    <row r="219" spans="2:16" ht="15.75">
+    <row r="219" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="P219" s="4"/>
     </row>
-    <row r="220" spans="2:16" ht="15.75">
+    <row r="220" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="P220" s="4"/>
     </row>
-    <row r="221" spans="2:16" ht="15.75">
+    <row r="221" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="P221" s="4"/>
     </row>
-    <row r="222" spans="2:16" ht="15.75">
+    <row r="222" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="P222" s="4"/>
     </row>
-    <row r="223" spans="2:16" ht="15.75">
+    <row r="223" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="P223" s="4"/>
     </row>
-    <row r="224" spans="2:16" ht="15.75">
+    <row r="224" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="P224" s="4"/>
     </row>
-    <row r="225" spans="2:16" ht="15.75">
+    <row r="225" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="P225" s="4"/>
     </row>
-    <row r="226" spans="2:16" ht="15.75">
+    <row r="226" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="P226" s="4"/>
     </row>
-    <row r="227" spans="2:16" ht="15.75">
+    <row r="227" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="P227" s="4"/>
     </row>
-    <row r="228" spans="2:16" ht="15.75">
+    <row r="228" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="P228" s="4"/>
     </row>
-    <row r="229" spans="2:16" ht="15.75">
+    <row r="229" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="P229" s="4"/>
     </row>
-    <row r="230" spans="2:16" ht="15.75">
+    <row r="230" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="P230" s="4"/>
     </row>
-    <row r="231" spans="2:16" ht="15.75">
+    <row r="231" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="P231" s="4"/>
     </row>
-    <row r="232" spans="2:16" ht="15.75">
+    <row r="232" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="P232" s="4"/>
     </row>
-    <row r="233" spans="2:16" ht="15.75">
+    <row r="233" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="P233" s="4"/>
     </row>
-    <row r="234" spans="2:16" ht="15.75">
+    <row r="234" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="P234" s="4"/>
     </row>
-    <row r="235" spans="2:16" ht="15.75">
+    <row r="235" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="P235" s="4"/>
     </row>
-    <row r="236" spans="2:16" ht="15.75">
+    <row r="236" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="P236" s="4"/>
     </row>
-    <row r="237" spans="2:16" ht="15.75">
+    <row r="237" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="P237" s="4"/>
     </row>
-    <row r="238" spans="2:16" ht="15.75">
+    <row r="238" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="P238" s="4"/>
     </row>
-    <row r="239" spans="2:16" ht="15.75">
+    <row r="239" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="P239" s="4"/>
     </row>
-    <row r="240" spans="2:16" ht="15.75">
+    <row r="240" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="P240" s="4"/>
     </row>
-    <row r="241" spans="2:16" ht="15.75">
+    <row r="241" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="P241" s="4"/>
     </row>
-    <row r="242" spans="2:16" ht="15.75">
+    <row r="242" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="P242" s="4"/>
     </row>
-    <row r="243" spans="2:16" ht="15.75">
+    <row r="243" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="2:16" ht="15.75">
+    <row r="244" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="2:16" ht="15.75">
+    <row r="245" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="2:16" ht="15.75">
+    <row r="246" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="2:16" ht="15.75">
+    <row r="247" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="2:16" ht="15.75">
+    <row r="248" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="2:16" ht="15.75">
+    <row r="249" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="2:16" ht="15.75">
+    <row r="250" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="2:16" ht="15.75">
+    <row r="251" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="2:16" ht="15.75">
+    <row r="252" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="2:16" ht="15.75">
+    <row r="253" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="2:16" ht="15.75">
+    <row r="254" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="2:16" ht="15.75">
+    <row r="255" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="2:16" ht="15.75">
+    <row r="256" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="2:4" ht="15.75">
+    <row r="257" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="2:4" ht="15.75">
+    <row r="258" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="2:4" ht="15.75">
+    <row r="259" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="2:4" ht="15.75">
+    <row r="260" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="2:4" ht="15.75">
+    <row r="261" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="2:4" ht="15.75">
+    <row r="262" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="2:4" ht="15.75">
+    <row r="263" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="2:4" ht="15.75">
+    <row r="264" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="2:4" ht="15.75">
+    <row r="265" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="2:4" ht="15.75">
+    <row r="266" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="2:4" ht="15.75">
+    <row r="267" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="2:4" ht="15.75">
+    <row r="268" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="2:4" ht="15.75">
+    <row r="269" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="2:4" ht="15.75">
+    <row r="270" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="2:4" ht="15.75">
+    <row r="271" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="2:4" ht="15.75">
+    <row r="272" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="2:4" ht="15.75">
+    <row r="273" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="2:4" ht="15.75">
+    <row r="274" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="2:4" ht="15.75">
+    <row r="275" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="2:4" ht="15.75">
+    <row r="276" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="2:4" ht="15.75">
+    <row r="277" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="2:4" ht="15.75">
+    <row r="278" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="2:4" ht="15.75">
+    <row r="279" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="2:4" ht="15.75">
+    <row r="280" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="2:4" ht="15.75">
+    <row r="281" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="2:4" ht="15.75">
+    <row r="282" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="2:4" ht="15.75">
+    <row r="283" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="2:4" ht="15.75">
+    <row r="284" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="2:4" ht="15.75">
+    <row r="285" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="2:4" ht="15.75">
+    <row r="286" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="2:4" ht="15.75">
+    <row r="287" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="2:4" ht="15.75">
+    <row r="288" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="2:4" ht="15.75">
+    <row r="289" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="2:4" ht="15.75">
+    <row r="290" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="2:4" ht="15.75">
+    <row r="291" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="2:4" ht="15.75">
+    <row r="292" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="2:4" ht="15.75">
+    <row r="293" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="2:4" ht="15.75">
+    <row r="294" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="2:4" ht="15.75">
+    <row r="295" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="2:4" ht="15.75">
+    <row r="296" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="2:4" ht="15.75">
+    <row r="297" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="2:4" ht="15.75">
+    <row r="298" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="2:4" ht="15.75">
+    <row r="299" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="2:4" ht="15.75">
+    <row r="300" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="2:4" ht="15.75">
+    <row r="301" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="2:4" ht="15.75">
+    <row r="302" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="2:4" ht="15.75">
+    <row r="303" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="2:4" ht="15.75">
+    <row r="304" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="2:4" ht="15.75">
+    <row r="305" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="2:4" ht="15.75">
+    <row r="306" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="2:4" ht="15.75">
+    <row r="307" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="2:4" ht="15.75">
+    <row r="308" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="2:4" ht="15.75">
+    <row r="309" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="2:4" ht="15.75">
+    <row r="310" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="2:4" ht="15.75">
+    <row r="311" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="2:4" ht="15.75">
+    <row r="312" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="2:4" ht="15.75">
+    <row r="313" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="2:4" ht="15.75">
+    <row r="314" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="2:4" ht="15.75">
+    <row r="315" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="2:4" ht="15.75">
+    <row r="316" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="2:4" ht="15.75">
+    <row r="317" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="2:4" ht="15.75">
+    <row r="318" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="2:4" ht="15.75">
+    <row r="319" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="2:4" ht="15.75">
+    <row r="320" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="2:4" ht="15.75">
+    <row r="321" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="2:4" ht="15.75">
+    <row r="322" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="2:4" ht="15.75">
+    <row r="323" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="2:4" ht="15.75">
+    <row r="324" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="2:4" ht="15.75">
+    <row r="325" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="2:4" ht="15.75">
+    <row r="326" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="2:4" ht="15.75">
+    <row r="327" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="2:4" ht="15.75">
+    <row r="328" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="2:4" ht="15.75">
+    <row r="329" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="2:4" ht="15.75">
+    <row r="330" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="2:4" ht="15.75">
+    <row r="331" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="2:4" ht="15.75">
+    <row r="332" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="2:4" ht="15.75">
+    <row r="333" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="2:4" ht="15.75">
+    <row r="334" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="2:4" ht="15.75">
+    <row r="335" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="2:4" ht="15.75">
+    <row r="336" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="2:4" ht="15.75">
+    <row r="337" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="2:4" ht="15.75">
+    <row r="338" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="2:4" ht="15.75">
+    <row r="339" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="2:4" ht="15.75">
+    <row r="340" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="2:4" ht="15.75">
+    <row r="341" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="2:4" ht="15.75">
+    <row r="342" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="2:4" ht="15.75">
+    <row r="343" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="2:4" ht="15.75">
+    <row r="344" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="2:4" ht="15.75">
+    <row r="345" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="2:4" ht="15.75">
+    <row r="346" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="2:4" ht="15.75">
+    <row r="347" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="2:4" ht="15.75">
+    <row r="348" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="2:4" ht="15.75">
+    <row r="349" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="2:4" ht="15.75">
+    <row r="350" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="2:4" ht="15.75">
+    <row r="351" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="2:4" ht="15.75">
+    <row r="352" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="2:4" ht="15.75">
+    <row r="353" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="2:4" ht="15.75">
+    <row r="354" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="2:4" ht="15.75">
+    <row r="355" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="2:4" ht="15.75">
+    <row r="356" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="2:4" ht="15.75">
+    <row r="357" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="2:4" ht="15.75">
+    <row r="358" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="2:4" ht="15.75">
+    <row r="359" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="2:4" ht="15.75">
+    <row r="360" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="2:4" ht="15.75">
+    <row r="361" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="2:4" ht="15.75">
+    <row r="362" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="2:4" ht="15.75">
+    <row r="363" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="2:4" ht="15.75">
+    <row r="364" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="2:4" ht="15.75">
+    <row r="365" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="2:4" ht="15.75">
+    <row r="366" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="2:4" ht="15.75">
+    <row r="367" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="2:4" ht="15.75">
+    <row r="368" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="2:4" ht="15.75">
+    <row r="369" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="2:4" ht="15.75">
+    <row r="370" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="2:4" ht="15.75">
+    <row r="371" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="2:4" ht="15.75">
+    <row r="372" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="2:4" ht="15.75">
+    <row r="373" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="2:4" ht="15.75">
+    <row r="374" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="2:4" ht="15.75">
+    <row r="375" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="2:4" ht="15.75">
+    <row r="376" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="2:4" ht="15.75">
+    <row r="377" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="2:4" ht="15.75">
+    <row r="378" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="2:4" ht="15.75">
+    <row r="379" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="2:4" ht="15.75">
+    <row r="380" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="2:4" ht="15.75">
+    <row r="381" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="2:4" ht="15.75">
+    <row r="382" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="2:4" ht="15.75">
+    <row r="383" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="2:4" ht="15.75">
+    <row r="384" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="2:4" ht="15.75">
+    <row r="385" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="2:4" ht="15.75">
+    <row r="386" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="2:4" ht="15.75">
+    <row r="387" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="2:4" ht="15.75">
+    <row r="388" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="2:4" ht="15.75">
+    <row r="389" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="2:4" ht="15.75">
+    <row r="390" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="2:4" ht="15.75">
+    <row r="391" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="2:4" ht="15.75">
+    <row r="392" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="2:4" ht="15.75">
+    <row r="393" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="2:4" ht="15.75">
+    <row r="394" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="2:4" ht="15.75">
+    <row r="395" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="2:4" ht="15.75">
+    <row r="396" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="2:4" ht="15.75">
+    <row r="397" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="2:4" ht="15.75">
+    <row r="398" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="2:4" ht="15.75">
+    <row r="399" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="2:4" ht="15.75">
+    <row r="400" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="2:4" ht="15.75">
+    <row r="401" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="2:4" ht="15.75">
+    <row r="402" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="2:4" ht="15.75">
+    <row r="403" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="2:4" ht="15.75">
+    <row r="404" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B404" s="2"/>
       <c r="C404" s="2"/>
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="2:4" ht="15.75">
+    <row r="405" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B405" s="2"/>
       <c r="C405" s="2"/>
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="2:4" ht="15.75">
+    <row r="406" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B406" s="2"/>
       <c r="C406" s="2"/>
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="2:4" ht="15.75">
+    <row r="407" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B407" s="2"/>
       <c r="C407" s="2"/>
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="2:4" ht="15.75">
+    <row r="408" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B408" s="2"/>
       <c r="C408" s="2"/>
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="2:4" ht="15.75">
+    <row r="409" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="2:4" ht="15.75">
+    <row r="410" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B410" s="2"/>
       <c r="C410" s="2"/>
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="2:4" ht="15.75">
+    <row r="411" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B411" s="2"/>
       <c r="C411" s="2"/>
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="2:4" ht="15.75">
+    <row r="412" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
       <c r="D412" s="2"/>

</xml_diff>

<commit_message>
Major performance in image processing
the images are not copied in high resolution but directly as thumbnails + updates in logging system
</commit_message>
<xml_diff>
--- a/SPPDATA_EX.xlsx
+++ b/SPPDATA_EX.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Garcilazo\Javascript_NodeJS\FAPOWebpage\02_Editing_Dynamic\PYTHON_Version\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8559A360-DD8E-413C-A833-BE356CAE8426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="SPECIES DATA" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>SPECIES</t>
   </si>
@@ -90,9 +84,6 @@
     <t>Galán-Sánchez</t>
   </si>
   <si>
-    <t>Salgueiro-Sepúlveda</t>
-  </si>
-  <si>
     <t>[urn:lsid:nmbe.ch:spidersp:009027]</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>TXV058</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 20-27.IX.2017: TXV058</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -120,18 +108,12 @@
     <t>TXV084</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 9-16.II.2018: TXV084</t>
-  </si>
-  <si>
     <t>Epilineutes sp02</t>
   </si>
   <si>
     <t>TXV085</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 16-22.V.2016: TXV085</t>
-  </si>
-  <si>
     <t>Chthonos sp01</t>
   </si>
   <si>
@@ -141,9 +123,6 @@
     <t>TXV573</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 20-27.IX.2017: TXV573</t>
-  </si>
-  <si>
     <t>Paulo Pantoja</t>
   </si>
   <si>
@@ -162,9 +141,6 @@
     <t>TXV083</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 9-16.II.2018: TXV083</t>
-  </si>
-  <si>
     <t>Theridiosoma sp01</t>
   </si>
   <si>
@@ -174,9 +150,6 @@
     <t>TXV082</t>
   </si>
   <si>
-    <t>Mexico: Veracruz, San Andres Tuxtla. Estacion de Biologia Tropical, Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates 18°34'56.1" N, 95°04'32.1" W. Alt. 217-172 m. Tropical Wet Forest. 9-16.II.2018: TXV082</t>
-  </si>
-  <si>
     <t>Phoroncidia sp01</t>
   </si>
   <si>
@@ -196,13 +169,19 @@
   </si>
   <si>
     <t>INVTUXV215</t>
+  </si>
+  <si>
+    <t>Mexico: Veracruz, Estacion de Biologia Tropical Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates: 18.58225, -95.07558333, 217-172 m. Tropical Wet Forest</t>
+  </si>
+  <si>
+    <t>Álvarez-Padilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,27 +335,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,24 +369,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -601,30 +544,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26171875" customWidth="1"/>
-    <col min="5" max="5" width="17.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.41796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -671,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -682,22 +628,22 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
+      <c r="I2" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -716,21 +662,21 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -739,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -761,21 +707,21 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -784,10 +730,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -806,21 +752,21 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -829,13 +775,13 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -844,40 +790,40 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -896,21 +842,21 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -919,10 +865,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -941,620 +887,620 @@
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16">
       <c r="A8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16">
       <c r="A9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16">
       <c r="A10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16">
       <c r="A11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:16">
       <c r="A12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16">
       <c r="A13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:16">
       <c r="A14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16">
       <c r="A15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16">
       <c r="A16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16">
       <c r="A17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16">
       <c r="A18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16">
       <c r="A19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16">
       <c r="A20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16">
       <c r="A21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16">
       <c r="A22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16">
       <c r="A23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16">
       <c r="A24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16">
       <c r="A25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:16">
       <c r="A26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:16">
       <c r="A27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:16">
       <c r="A28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:16">
       <c r="A29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16">
       <c r="A30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16">
       <c r="A31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:16">
       <c r="A32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:16">
       <c r="A33" s="3"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:16">
       <c r="A34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:16">
       <c r="A35" s="4"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:16">
       <c r="A36" s="4"/>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:16">
       <c r="A37" s="4"/>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:16">
       <c r="A38" s="4"/>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:16">
       <c r="A39" s="4"/>
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:16">
       <c r="A40" s="4"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:16">
       <c r="A41" s="4"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:16">
       <c r="A42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:16">
       <c r="A43" s="4"/>
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:16">
       <c r="A44" s="4"/>
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:16">
       <c r="A45" s="4"/>
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:16">
       <c r="A46" s="4"/>
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:16">
       <c r="A47" s="4"/>
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:16">
       <c r="A48" s="4"/>
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:16">
       <c r="A49" s="4"/>
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:16">
       <c r="A50" s="4"/>
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:16">
       <c r="A51" s="4"/>
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:16">
       <c r="A52" s="4"/>
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:16">
       <c r="A53" s="4"/>
       <c r="P53" s="4"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:16">
       <c r="A54" s="4"/>
       <c r="P54" s="4"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:16">
       <c r="A55" s="4"/>
       <c r="P55" s="4"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:16">
       <c r="A56" s="4"/>
       <c r="P56" s="4"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:16">
       <c r="A57" s="3"/>
       <c r="P57" s="4"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:16">
       <c r="A58" s="4"/>
       <c r="P58" s="3"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:16">
       <c r="A59" s="4"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:16">
       <c r="A60" s="4"/>
       <c r="P60" s="4"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:16">
       <c r="A61" s="4"/>
       <c r="P61" s="4"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:16">
       <c r="A62" s="4"/>
       <c r="P62" s="4"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:16">
       <c r="A63" s="4"/>
       <c r="P63" s="4"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:16">
       <c r="A64" s="4"/>
       <c r="P64" s="4"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:16">
       <c r="A65" s="4"/>
       <c r="P65" s="4"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:16">
       <c r="A66" s="4"/>
       <c r="P66" s="4"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:16">
       <c r="A67" s="4"/>
       <c r="P67" s="4"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:16">
       <c r="A68" s="4"/>
       <c r="P68" s="4"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:16">
       <c r="A69" s="4"/>
       <c r="P69" s="4"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:16">
       <c r="A70" s="4"/>
       <c r="P70" s="4"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:16">
       <c r="A71" s="4"/>
       <c r="P71" s="4"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:16">
       <c r="A72" s="4"/>
       <c r="P72" s="4"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:16">
       <c r="A73" s="4"/>
       <c r="P73" s="4"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:16">
       <c r="A74" s="4"/>
       <c r="P74" s="4"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:16">
       <c r="A75" s="4"/>
       <c r="P75" s="4"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:16">
       <c r="A76" s="4"/>
       <c r="P76" s="4"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:16">
       <c r="A77" s="4"/>
       <c r="P77" s="4"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:16">
       <c r="A78" s="4"/>
       <c r="P78" s="4"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:16">
       <c r="A79" s="4"/>
       <c r="P79" s="4"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:16">
       <c r="A80" s="4"/>
       <c r="P80" s="4"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:16">
       <c r="A81" s="4"/>
       <c r="P81" s="4"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:16">
       <c r="A82" s="4"/>
       <c r="P82" s="4"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:16">
       <c r="A83" s="4"/>
       <c r="P83" s="4"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:16">
       <c r="A84" s="4"/>
       <c r="P84" s="4"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:16">
       <c r="A85" s="4"/>
       <c r="P85" s="4"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:16">
       <c r="A86" s="4"/>
       <c r="P86" s="4"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:16">
       <c r="A87" s="4"/>
       <c r="P87" s="4"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:16">
       <c r="A88" s="4"/>
       <c r="P88" s="4"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:16">
       <c r="A89" s="4"/>
       <c r="P89" s="3"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:16">
       <c r="A90" s="4"/>
       <c r="P90" s="4"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:16">
       <c r="A91" s="4"/>
       <c r="P91" s="4"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:16">
       <c r="A92" s="4"/>
       <c r="P92" s="4"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:16">
       <c r="A93" s="4"/>
       <c r="P93" s="4"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:16">
       <c r="A94" s="4"/>
       <c r="P94" s="4"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:16">
       <c r="A95" s="4"/>
       <c r="P95" s="4"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:16">
       <c r="A96" s="4"/>
       <c r="P96" s="4"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:16">
       <c r="A97" s="4"/>
       <c r="P97" s="4"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:16">
       <c r="A98" s="4"/>
       <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:16">
       <c r="A99" s="4"/>
       <c r="P99" s="4"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:16">
       <c r="A100" s="4"/>
       <c r="P100" s="4"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:16">
       <c r="A101" s="4"/>
       <c r="P101" s="4"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:16">
       <c r="A102" s="4"/>
       <c r="P102" s="4"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:16">
       <c r="A103" s="4"/>
       <c r="P103" s="4"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:16">
       <c r="A104" s="4"/>
       <c r="P104" s="4"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:16">
       <c r="A105" s="4"/>
       <c r="P105" s="4"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:16">
       <c r="A106" s="4"/>
       <c r="P106" s="4"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:16">
       <c r="A107" s="4"/>
       <c r="P107" s="4"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:16">
       <c r="A108" s="4"/>
       <c r="P108" s="4"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:16">
       <c r="A109" s="4"/>
       <c r="P109" s="4"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:16">
       <c r="A110" s="4"/>
       <c r="P110" s="4"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:16">
       <c r="A111" s="4"/>
       <c r="P111" s="4"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:16">
       <c r="A112" s="4"/>
       <c r="P112" s="4"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:16">
       <c r="A113" s="4"/>
       <c r="P113" s="4"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:16">
       <c r="A114" s="4"/>
       <c r="P114" s="4"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:16">
       <c r="A115" s="4"/>
       <c r="P115" s="4"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:16">
       <c r="A116" s="4"/>
       <c r="P116" s="4"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:16">
       <c r="A117" s="4"/>
       <c r="P117" s="4"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:16">
       <c r="A118" s="4"/>
       <c r="P118" s="4"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:16">
       <c r="A119" s="4"/>
       <c r="P119" s="4"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:16">
       <c r="A120" s="4"/>
       <c r="P120" s="4"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:16">
       <c r="A121" s="4"/>
       <c r="P121" s="4"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:16">
       <c r="A122" s="4"/>
       <c r="P122" s="4"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:16">
       <c r="A123" s="4"/>
       <c r="P123" s="4"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:16">
       <c r="A124" s="4"/>
       <c r="P124" s="4"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:16">
       <c r="A125" s="4"/>
       <c r="P125" s="4"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:16">
       <c r="A126" s="4"/>
       <c r="P126" s="4"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:16">
       <c r="A127" s="4"/>
       <c r="P127" s="4"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:16">
       <c r="A128" s="4"/>
       <c r="P128" s="4"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:16">
       <c r="A129" s="4"/>
       <c r="P129" s="4"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:16">
       <c r="A130" s="4"/>
       <c r="P130" s="4"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:16">
       <c r="A131" s="4"/>
       <c r="P131" s="4"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:16">
       <c r="A132" s="4"/>
       <c r="P132" s="4"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:16">
       <c r="A133" s="4"/>
       <c r="P133" s="4"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:16">
       <c r="A134" s="4"/>
       <c r="P134" s="4"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:16">
       <c r="A135" s="4"/>
       <c r="P135" s="4"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:16">
       <c r="A136" s="4"/>
       <c r="P136" s="4"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:16">
       <c r="A137" s="4"/>
       <c r="P137" s="4"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:16">
       <c r="A138" s="4"/>
       <c r="P138" s="4"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:16">
       <c r="A139" s="4"/>
       <c r="P139" s="4"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:16">
       <c r="A140" s="4"/>
       <c r="P140" s="4"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:16">
       <c r="A141" s="4"/>
       <c r="P141" s="4"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:16">
       <c r="A142" s="4"/>
       <c r="P142" s="4"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:16">
       <c r="A143" s="4"/>
       <c r="P143" s="4"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:16">
       <c r="P144" s="4"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:1">
       <c r="A150" s="4"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:1">
       <c r="A151" s="4"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:1">
       <c r="A152" s="4"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:1">
       <c r="A153" s="4"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:1">
       <c r="A154" s="4"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:1">
       <c r="A155" s="4"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:1">
       <c r="A156" s="4"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:1">
       <c r="A157" s="4"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:1">
       <c r="A158" s="4"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:1">
       <c r="A159" s="4"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:1">
       <c r="A160" s="4"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:13">
       <c r="A161" s="4"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:13">
       <c r="A162" s="4"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:13">
       <c r="A163" s="4"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:13">
       <c r="A164" s="4"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:13">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:13">
       <c r="A166" s="4"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:13">
       <c r="A167" s="4"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:13">
       <c r="A168" s="4"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:13">
       <c r="A169" s="4"/>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:13">
       <c r="A170" s="4"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:13">
       <c r="A171" s="4"/>
     </row>
-    <row r="172" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
+    <row r="172" spans="1:13" ht="16.5">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -1569,7 +1515,7 @@
       <c r="L172" s="5"/>
       <c r="M172" s="5"/>
     </row>
-    <row r="173" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
+    <row r="173" spans="1:13" ht="16.5">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -1584,7 +1530,7 @@
       <c r="L173" s="5"/>
       <c r="M173" s="5"/>
     </row>
-    <row r="174" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
+    <row r="174" spans="1:13" ht="16.5">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -1599,7 +1545,7 @@
       <c r="L174" s="5"/>
       <c r="M174" s="5"/>
     </row>
-    <row r="175" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
+    <row r="175" spans="1:13" ht="16.5">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -1614,7 +1560,7 @@
       <c r="L175" s="5"/>
       <c r="M175" s="5"/>
     </row>
-    <row r="176" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
+    <row r="176" spans="1:13" ht="16.5">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -1628,7 +1574,7 @@
       <c r="L176" s="5"/>
       <c r="M176" s="5"/>
     </row>
-    <row r="177" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
+    <row r="177" spans="1:13" ht="16.5">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -1642,7 +1588,7 @@
       <c r="L177" s="5"/>
       <c r="M177" s="5"/>
     </row>
-    <row r="178" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
+    <row r="178" spans="1:13" ht="16.5">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -1656,1203 +1602,1203 @@
       <c r="L178" s="5"/>
       <c r="M178" s="5"/>
     </row>
-    <row r="179" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:13" ht="15.75">
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:13" ht="15.75">
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:13" ht="15.75">
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:13" ht="15.75">
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:13" ht="15.75">
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:13" ht="15.75">
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:13" ht="15.75">
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:13" ht="15.75">
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:13" ht="15.75">
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:13" ht="15.75">
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:13" ht="15.75">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:13" ht="15.75">
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:13" ht="15.75">
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:13" ht="15.75">
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="2:4" ht="15.75">
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="2:4" ht="15.75">
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="2:4" ht="15.75">
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="2:4" ht="15.75">
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="2:4" ht="15.75">
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="2:4" ht="15.75">
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="2:4" ht="15.75">
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="2:4" ht="15.75">
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="2:4" ht="15.75">
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="2:4" ht="15.75">
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="2:4" ht="15.75">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="2:4" ht="15.75">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="2:4" ht="15.75">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="2:4" ht="15.75">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="2:4" ht="15.75">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="2:4" ht="15.75">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="2:16" ht="15.75">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="2:16" ht="15.75">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="2:16" ht="15.75">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="2:16" ht="15.75">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="P212" s="4"/>
     </row>
-    <row r="213" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="2:16" ht="15.75">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="P213" s="4"/>
     </row>
-    <row r="214" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="2:16" ht="15.75">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="P214" s="4"/>
     </row>
-    <row r="215" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="2:16" ht="15.75">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="P215" s="4"/>
     </row>
-    <row r="216" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="2:16" ht="15.75">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="P216" s="4"/>
     </row>
-    <row r="217" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="2:16" ht="15.75">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="P217" s="4"/>
     </row>
-    <row r="218" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="2:16" ht="15.75">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="P218" s="4"/>
     </row>
-    <row r="219" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="2:16" ht="15.75">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="P219" s="4"/>
     </row>
-    <row r="220" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="2:16" ht="15.75">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="P220" s="4"/>
     </row>
-    <row r="221" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="2:16" ht="15.75">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="P221" s="4"/>
     </row>
-    <row r="222" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="2:16" ht="15.75">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="P222" s="4"/>
     </row>
-    <row r="223" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="2:16" ht="15.75">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="P223" s="4"/>
     </row>
-    <row r="224" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="2:16" ht="15.75">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="P224" s="4"/>
     </row>
-    <row r="225" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="2:16" ht="15.75">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="P225" s="4"/>
     </row>
-    <row r="226" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="2:16" ht="15.75">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="P226" s="4"/>
     </row>
-    <row r="227" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="2:16" ht="15.75">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="P227" s="4"/>
     </row>
-    <row r="228" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="2:16" ht="15.75">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="P228" s="4"/>
     </row>
-    <row r="229" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="2:16" ht="15.75">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="P229" s="4"/>
     </row>
-    <row r="230" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="2:16" ht="15.75">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="P230" s="4"/>
     </row>
-    <row r="231" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="2:16" ht="15.75">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="P231" s="4"/>
     </row>
-    <row r="232" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="2:16" ht="15.75">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="P232" s="4"/>
     </row>
-    <row r="233" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="2:16" ht="15.75">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="P233" s="4"/>
     </row>
-    <row r="234" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="2:16" ht="15.75">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="P234" s="4"/>
     </row>
-    <row r="235" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="2:16" ht="15.75">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="P235" s="4"/>
     </row>
-    <row r="236" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="2:16" ht="15.75">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="P236" s="4"/>
     </row>
-    <row r="237" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="2:16" ht="15.75">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="P237" s="4"/>
     </row>
-    <row r="238" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="2:16" ht="15.75">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="P238" s="4"/>
     </row>
-    <row r="239" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="2:16" ht="15.75">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="P239" s="4"/>
     </row>
-    <row r="240" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="2:16" ht="15.75">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="P240" s="4"/>
     </row>
-    <row r="241" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="2:16" ht="15.75">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="P241" s="4"/>
     </row>
-    <row r="242" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="2:16" ht="15.75">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="P242" s="4"/>
     </row>
-    <row r="243" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="2:16" ht="15.75">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="2:16" ht="15.75">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="2:16" ht="15.75">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="2:16" ht="15.75">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="2:16" ht="15.75">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="2:16" ht="15.75">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="2:16" ht="15.75">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="2:16" ht="15.75">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="2:16" ht="15.75">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="2:16" ht="15.75">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="2:16" ht="15.75">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="2:16" ht="15.75">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="2:16" ht="15.75">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="2:16" ht="15.75">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="2:4" ht="15.75">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="2:4" ht="15.75">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="2:4" ht="15.75">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="2:4" ht="15.75">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="2:4" ht="15.75">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="2:4" ht="15.75">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="2:4" ht="15.75">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="2:4" ht="15.75">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="2:4" ht="15.75">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="2:4" ht="15.75">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="2:4" ht="15.75">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="2:4" ht="15.75">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="2:4" ht="15.75">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="2:4" ht="15.75">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="2:4" ht="15.75">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="2:4" ht="15.75">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="2:4" ht="15.75">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="2:4" ht="15.75">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="2:4" ht="15.75">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="2:4" ht="15.75">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="2:4" ht="15.75">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="2:4" ht="15.75">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="2:4" ht="15.75">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="2:4" ht="15.75">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="2:4" ht="15.75">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="2:4" ht="15.75">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="2:4" ht="15.75">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="2:4" ht="15.75">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="2:4" ht="15.75">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="2:4" ht="15.75">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="2:4" ht="15.75">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="2:4" ht="15.75">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="2:4" ht="15.75">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="2:4" ht="15.75">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="2:4" ht="15.75">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="2:4" ht="15.75">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="2:4" ht="15.75">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="2:4" ht="15.75">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="2:4" ht="15.75">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="2:4" ht="15.75">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="2:4" ht="15.75">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="2:4" ht="15.75">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="2:4" ht="15.75">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="2:4" ht="15.75">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="2:4" ht="15.75">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="2:4" ht="15.75">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="2:4" ht="15.75">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="2:4" ht="15.75">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="2:4" ht="15.75">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="2:4" ht="15.75">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="2:4" ht="15.75">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="2:4" ht="15.75">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="2:4" ht="15.75">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="2:4" ht="15.75">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="2:4" ht="15.75">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="2:4" ht="15.75">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="2:4" ht="15.75">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="2:4" ht="15.75">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="2:4" ht="15.75">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="2:4" ht="15.75">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="2:4" ht="15.75">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="2:4" ht="15.75">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="2:4" ht="15.75">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="2:4" ht="15.75">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="2:4" ht="15.75">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="2:4" ht="15.75">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="2:4" ht="15.75">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="2:4" ht="15.75">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="2:4" ht="15.75">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="2:4" ht="15.75">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="2:4" ht="15.75">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="2:4" ht="15.75">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="2:4" ht="15.75">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="2:4" ht="15.75">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="2:4" ht="15.75">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="2:4" ht="15.75">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="2:4" ht="15.75">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="2:4" ht="15.75">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="2:4" ht="15.75">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="2:4" ht="15.75">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="2:4" ht="15.75">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="2:4" ht="15.75">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="2:4" ht="15.75">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="2:4" ht="15.75">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="2:4" ht="15.75">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="2:4" ht="15.75">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="2:4" ht="15.75">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="2:4" ht="15.75">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="2:4" ht="15.75">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="2:4" ht="15.75">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="2:4" ht="15.75">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="2:4" ht="15.75">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="2:4" ht="15.75">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="2:4" ht="15.75">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="2:4" ht="15.75">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="2:4" ht="15.75">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="2:4" ht="15.75">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="2:4" ht="15.75">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="2:4" ht="15.75">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="2:4" ht="15.75">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="2:4" ht="15.75">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="2:4" ht="15.75">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="2:4" ht="15.75">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="2:4" ht="15.75">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="2:4" ht="15.75">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="2:4" ht="15.75">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="2:4" ht="15.75">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="2:4" ht="15.75">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="2:4" ht="15.75">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="2:4" ht="15.75">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="2:4" ht="15.75">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="2:4" ht="15.75">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="2:4" ht="15.75">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="2:4" ht="15.75">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="2:4" ht="15.75">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="2:4" ht="15.75">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="2:4" ht="15.75">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="2:4" ht="15.75">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="2:4" ht="15.75">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="2:4" ht="15.75">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="2:4" ht="15.75">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="2:4" ht="15.75">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="2:4" ht="15.75">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="2:4" ht="15.75">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="2:4" ht="15.75">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="2:4" ht="15.75">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="2:4" ht="15.75">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="2:4" ht="15.75">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="2:4" ht="15.75">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="2:4" ht="15.75">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="2:4" ht="15.75">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="2:4" ht="15.75">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="2:4" ht="15.75">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="2:4" ht="15.75">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="2:4" ht="15.75">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="2:4" ht="15.75">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="2:4" ht="15.75">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="2:4" ht="15.75">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="2:4" ht="15.75">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="2:4" ht="15.75">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="2:4" ht="15.75">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="2:4" ht="15.75">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="2:4" ht="15.75">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="2:4" ht="15.75">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="2:4" ht="15.75">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="2:4" ht="15.75">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="2:4" ht="15.75">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="2:4" ht="15.75">
       <c r="B404" s="2"/>
       <c r="C404" s="2"/>
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="2:4" ht="15.75">
       <c r="B405" s="2"/>
       <c r="C405" s="2"/>
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="2:4" ht="15.75">
       <c r="B406" s="2"/>
       <c r="C406" s="2"/>
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="2:4" ht="15.75">
       <c r="B407" s="2"/>
       <c r="C407" s="2"/>
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="2:4" ht="15.75">
       <c r="B408" s="2"/>
       <c r="C408" s="2"/>
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="2:4" ht="15.75">
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="2:4" ht="15.75">
       <c r="B410" s="2"/>
       <c r="C410" s="2"/>
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="2:4" ht="15.75">
       <c r="B411" s="2"/>
       <c r="C411" s="2"/>
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="2:4" ht="15.75">
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
       <c r="D412" s="2"/>

</xml_diff>

<commit_message>
Initial checkup evaluates critical errors
</commit_message>
<xml_diff>
--- a/SPPDATA_EX.xlsx
+++ b/SPPDATA_EX.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Garcilazo\Javascript_NodeJS\FAPOWebpage\02_Editing_Dynamic\PYTHON_Version\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA710B4-5593-4CFA-AB5F-FBD249661C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPECIES DATA" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -93,95 +88,95 @@
     <t>Belize</t>
   </si>
   <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Epilineutes sp01</t>
+  </si>
+  <si>
+    <t>[urn:lsid:nmbe.ch:spidergen:00739]</t>
+  </si>
+  <si>
+    <t>TXV084</t>
+  </si>
+  <si>
+    <t>Epilineutes sp02</t>
+  </si>
+  <si>
+    <t>TXV085</t>
+  </si>
+  <si>
+    <t>Chthonos sp01</t>
+  </si>
+  <si>
+    <t>[urn:lsid:nmbe.ch:spidergen:00737]</t>
+  </si>
+  <si>
+    <t>TXV573</t>
+  </si>
+  <si>
+    <t>Paulo Pantoja</t>
+  </si>
+  <si>
+    <t>Misidentified as &lt;I&gt;Phoroncidia sp01&lt;/I&gt; in &amp;Aacute;varez-Padilla et al. 2020.</t>
+  </si>
+  <si>
+    <t>Theridiosoma chiripa</t>
+  </si>
+  <si>
+    <t>[urn:lsid:nmbe.ch:spidersp:039839]</t>
+  </si>
+  <si>
+    <t>Rodrigues &amp; Ott, 2005</t>
+  </si>
+  <si>
+    <t>TXV083</t>
+  </si>
+  <si>
+    <t>Theridiosoma sp01</t>
+  </si>
+  <si>
+    <t>[urn:lsid:nmbe.ch:spidergen:00744]</t>
+  </si>
+  <si>
+    <t>TXV082</t>
+  </si>
+  <si>
+    <t>Phoroncidia sp01</t>
+  </si>
+  <si>
+    <t>INVTUXV212</t>
+  </si>
+  <si>
+    <t>INVTUXV213</t>
+  </si>
+  <si>
+    <t>INVTUXV214</t>
+  </si>
+  <si>
+    <t>INVTUXV216</t>
+  </si>
+  <si>
+    <t>INVTUXV217</t>
+  </si>
+  <si>
+    <t>Mexico: Veracruz, Estacion de Biologia Tropical Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates: 18.58225, -95.07558333, 217-172 m. Tropical Wet Forest</t>
+  </si>
+  <si>
+    <t>Álvarez-Padilla</t>
+  </si>
+  <si>
     <t>TXV058</t>
   </si>
   <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Epilineutes sp01</t>
-  </si>
-  <si>
-    <t>[urn:lsid:nmbe.ch:spidergen:00739]</t>
-  </si>
-  <si>
-    <t>TXV084</t>
-  </si>
-  <si>
-    <t>Epilineutes sp02</t>
-  </si>
-  <si>
-    <t>TXV085</t>
-  </si>
-  <si>
-    <t>Chthonos sp01</t>
-  </si>
-  <si>
-    <t>[urn:lsid:nmbe.ch:spidergen:00737]</t>
-  </si>
-  <si>
-    <t>TXV573</t>
-  </si>
-  <si>
-    <t>Paulo Pantoja</t>
-  </si>
-  <si>
-    <t>Misidentified as &lt;I&gt;Phoroncidia sp01&lt;/I&gt; in &amp;Aacute;varez-Padilla et al. 2020.</t>
-  </si>
-  <si>
-    <t>Theridiosoma chiripa</t>
-  </si>
-  <si>
-    <t>[urn:lsid:nmbe.ch:spidersp:039839]</t>
-  </si>
-  <si>
-    <t>Rodrigues &amp; Ott, 2005</t>
-  </si>
-  <si>
-    <t>TXV083</t>
-  </si>
-  <si>
-    <t>Theridiosoma sp01</t>
-  </si>
-  <si>
-    <t>[urn:lsid:nmbe.ch:spidergen:00744]</t>
-  </si>
-  <si>
-    <t>TXV082</t>
-  </si>
-  <si>
-    <t>Phoroncidia sp01</t>
-  </si>
-  <si>
-    <t>INVTUXV212</t>
-  </si>
-  <si>
-    <t>INVTUXV213</t>
-  </si>
-  <si>
-    <t>INVTUXV214</t>
-  </si>
-  <si>
-    <t>INVTUXV216</t>
-  </si>
-  <si>
-    <t>INVTUXV217</t>
-  </si>
-  <si>
     <t>INVTUXV215</t>
-  </si>
-  <si>
-    <t>Mexico: Veracruz, Estacion de Biologia Tropical Los Tuxtlas IB-UNAM. Plot 1 ha. Central Coordinates: 18.58225, -95.07558333, 217-172 m. Tropical Wet Forest</t>
-  </si>
-  <si>
-    <t>Álvarez-Padilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,9 +330,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,6 +382,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -544,33 +575,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.68359375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.68359375" customWidth="1"/>
+    <col min="4" max="4" width="17.68359375" customWidth="1"/>
+    <col min="5" max="5" width="33.578125" customWidth="1"/>
+    <col min="6" max="6" width="21.68359375" customWidth="1"/>
+    <col min="7" max="7" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.68359375" customWidth="1"/>
+    <col min="10" max="10" width="22.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83984375" customWidth="1"/>
+    <col min="14" max="14" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75">
+    <row r="1" spans="1:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -617,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -628,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -640,10 +671,10 @@
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -662,21 +693,21 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -685,10 +716,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -707,21 +738,21 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -730,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -752,21 +783,21 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -775,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
         <v>31</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -790,40 +821,40 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -842,21 +873,21 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -865,10 +896,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -887,620 +918,620 @@
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4"/>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4"/>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4"/>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4"/>
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4"/>
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4"/>
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4"/>
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4"/>
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4"/>
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4"/>
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4"/>
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4"/>
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4"/>
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4"/>
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4"/>
       <c r="P53" s="4"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4"/>
       <c r="P54" s="4"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4"/>
       <c r="P55" s="4"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4"/>
       <c r="P56" s="4"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3"/>
       <c r="P57" s="4"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4"/>
       <c r="P58" s="3"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4"/>
       <c r="P60" s="4"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4"/>
       <c r="P61" s="4"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="4"/>
       <c r="P62" s="4"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="4"/>
       <c r="P63" s="4"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="4"/>
       <c r="P64" s="4"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="4"/>
       <c r="P65" s="4"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="4"/>
       <c r="P66" s="4"/>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="4"/>
       <c r="P67" s="4"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="4"/>
       <c r="P68" s="4"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4"/>
       <c r="P69" s="4"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4"/>
       <c r="P70" s="4"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4"/>
       <c r="P71" s="4"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="4"/>
       <c r="P72" s="4"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4"/>
       <c r="P73" s="4"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4"/>
       <c r="P74" s="4"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="4"/>
       <c r="P75" s="4"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="4"/>
       <c r="P76" s="4"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="4"/>
       <c r="P77" s="4"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="4"/>
       <c r="P78" s="4"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4"/>
       <c r="P79" s="4"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4"/>
       <c r="P80" s="4"/>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="4"/>
       <c r="P81" s="4"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="4"/>
       <c r="P82" s="4"/>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="4"/>
       <c r="P83" s="4"/>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4"/>
       <c r="P84" s="4"/>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4"/>
       <c r="P85" s="4"/>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4"/>
       <c r="P86" s="4"/>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4"/>
       <c r="P87" s="4"/>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4"/>
       <c r="P88" s="4"/>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4"/>
       <c r="P89" s="3"/>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="4"/>
       <c r="P90" s="4"/>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="4"/>
       <c r="P91" s="4"/>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4"/>
       <c r="P92" s="4"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="4"/>
       <c r="P93" s="4"/>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="4"/>
       <c r="P94" s="4"/>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4"/>
       <c r="P95" s="4"/>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4"/>
       <c r="P96" s="4"/>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="4"/>
       <c r="P97" s="4"/>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="4"/>
       <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="4"/>
       <c r="P99" s="4"/>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4"/>
       <c r="P100" s="4"/>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4"/>
       <c r="P101" s="4"/>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="4"/>
       <c r="P102" s="4"/>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4"/>
       <c r="P103" s="4"/>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="4"/>
       <c r="P104" s="4"/>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4"/>
       <c r="P105" s="4"/>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="4"/>
       <c r="P106" s="4"/>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4"/>
       <c r="P107" s="4"/>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4"/>
       <c r="P108" s="4"/>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="4"/>
       <c r="P109" s="4"/>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="4"/>
       <c r="P110" s="4"/>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4"/>
       <c r="P111" s="4"/>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="4"/>
       <c r="P112" s="4"/>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="4"/>
       <c r="P113" s="4"/>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="4"/>
       <c r="P114" s="4"/>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="4"/>
       <c r="P115" s="4"/>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="4"/>
       <c r="P116" s="4"/>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="4"/>
       <c r="P117" s="4"/>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="4"/>
       <c r="P118" s="4"/>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="4"/>
       <c r="P119" s="4"/>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="4"/>
       <c r="P120" s="4"/>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="4"/>
       <c r="P121" s="4"/>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="4"/>
       <c r="P122" s="4"/>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="4"/>
       <c r="P123" s="4"/>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="4"/>
       <c r="P124" s="4"/>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="4"/>
       <c r="P125" s="4"/>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="4"/>
       <c r="P126" s="4"/>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4"/>
       <c r="P127" s="4"/>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="4"/>
       <c r="P128" s="4"/>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="4"/>
       <c r="P129" s="4"/>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="4"/>
       <c r="P130" s="4"/>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="4"/>
       <c r="P131" s="4"/>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="4"/>
       <c r="P132" s="4"/>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="4"/>
       <c r="P133" s="4"/>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="4"/>
       <c r="P134" s="4"/>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="4"/>
       <c r="P135" s="4"/>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="4"/>
       <c r="P136" s="4"/>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="4"/>
       <c r="P137" s="4"/>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="4"/>
       <c r="P138" s="4"/>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="4"/>
       <c r="P139" s="4"/>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="4"/>
       <c r="P140" s="4"/>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="4"/>
       <c r="P141" s="4"/>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="4"/>
       <c r="P142" s="4"/>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="4"/>
       <c r="P143" s="4"/>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="P144" s="4"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="4"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="4"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="4"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="4"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="4"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="4"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="4"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="4"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="4"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="4"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="4"/>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="4"/>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="4"/>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="4"/>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="4"/>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="4"/>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="4"/>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="4"/>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="4"/>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="4"/>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="4"/>
     </row>
-    <row r="172" spans="1:13" ht="16.5">
+    <row r="172" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -1515,7 +1546,7 @@
       <c r="L172" s="5"/>
       <c r="M172" s="5"/>
     </row>
-    <row r="173" spans="1:13" ht="16.5">
+    <row r="173" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -1530,7 +1561,7 @@
       <c r="L173" s="5"/>
       <c r="M173" s="5"/>
     </row>
-    <row r="174" spans="1:13" ht="16.5">
+    <row r="174" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -1545,7 +1576,7 @@
       <c r="L174" s="5"/>
       <c r="M174" s="5"/>
     </row>
-    <row r="175" spans="1:13" ht="16.5">
+    <row r="175" spans="1:13" ht="15.9" x14ac:dyDescent="0.7">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -1560,7 +1591,7 @@
       <c r="L175" s="5"/>
       <c r="M175" s="5"/>
     </row>
-    <row r="176" spans="1:13" ht="16.5">
+    <row r="176" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -1574,7 +1605,7 @@
       <c r="L176" s="5"/>
       <c r="M176" s="5"/>
     </row>
-    <row r="177" spans="1:13" ht="16.5">
+    <row r="177" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -1588,7 +1619,7 @@
       <c r="L177" s="5"/>
       <c r="M177" s="5"/>
     </row>
-    <row r="178" spans="1:13" ht="16.5">
+    <row r="178" spans="1:13" ht="16.2" x14ac:dyDescent="0.7">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -1602,1203 +1633,1203 @@
       <c r="L178" s="5"/>
       <c r="M178" s="5"/>
     </row>
-    <row r="179" spans="1:13" ht="15.75">
+    <row r="179" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="1:13" ht="15.75">
+    <row r="180" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="1:13" ht="15.75">
+    <row r="181" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="1:13" ht="15.75">
+    <row r="182" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="1:13" ht="15.75">
+    <row r="183" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="1:13" ht="15.75">
+    <row r="184" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="1:13" ht="15.75">
+    <row r="185" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="1:13" ht="15.75">
+    <row r="186" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="1:13" ht="15.75">
+    <row r="187" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="1:13" ht="15.75">
+    <row r="188" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="1:13" ht="15.75">
+    <row r="189" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="1:13" ht="15.75">
+    <row r="190" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="1:13" ht="15.75">
+    <row r="191" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="1:13" ht="15.75">
+    <row r="192" spans="1:13" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="2:4" ht="15.75">
+    <row r="193" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="2:4" ht="15.75">
+    <row r="194" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="2:4" ht="15.75">
+    <row r="195" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="2:4" ht="15.75">
+    <row r="196" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="2:4" ht="15.75">
+    <row r="197" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="2:4" ht="15.75">
+    <row r="198" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="2:4" ht="15.75">
+    <row r="199" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="2:4" ht="15.75">
+    <row r="200" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="2:4" ht="15.75">
+    <row r="201" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="2:4" ht="15.75">
+    <row r="202" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="2:4" ht="15.75">
+    <row r="203" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="2:4" ht="15.75">
+    <row r="204" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="2:4" ht="15.75">
+    <row r="205" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="2:4" ht="15.75">
+    <row r="206" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="2:4" ht="15.75">
+    <row r="207" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="2:4" ht="15.75">
+    <row r="208" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="2:16" ht="15.75">
+    <row r="209" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="2:16" ht="15.75">
+    <row r="210" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="2:16" ht="15.75">
+    <row r="211" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="2:16" ht="15.75">
+    <row r="212" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="P212" s="4"/>
     </row>
-    <row r="213" spans="2:16" ht="15.75">
+    <row r="213" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="P213" s="4"/>
     </row>
-    <row r="214" spans="2:16" ht="15.75">
+    <row r="214" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="P214" s="4"/>
     </row>
-    <row r="215" spans="2:16" ht="15.75">
+    <row r="215" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="P215" s="4"/>
     </row>
-    <row r="216" spans="2:16" ht="15.75">
+    <row r="216" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="P216" s="4"/>
     </row>
-    <row r="217" spans="2:16" ht="15.75">
+    <row r="217" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="P217" s="4"/>
     </row>
-    <row r="218" spans="2:16" ht="15.75">
+    <row r="218" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="P218" s="4"/>
     </row>
-    <row r="219" spans="2:16" ht="15.75">
+    <row r="219" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="P219" s="4"/>
     </row>
-    <row r="220" spans="2:16" ht="15.75">
+    <row r="220" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="P220" s="4"/>
     </row>
-    <row r="221" spans="2:16" ht="15.75">
+    <row r="221" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="P221" s="4"/>
     </row>
-    <row r="222" spans="2:16" ht="15.75">
+    <row r="222" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="P222" s="4"/>
     </row>
-    <row r="223" spans="2:16" ht="15.75">
+    <row r="223" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="P223" s="4"/>
     </row>
-    <row r="224" spans="2:16" ht="15.75">
+    <row r="224" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="P224" s="4"/>
     </row>
-    <row r="225" spans="2:16" ht="15.75">
+    <row r="225" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="P225" s="4"/>
     </row>
-    <row r="226" spans="2:16" ht="15.75">
+    <row r="226" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="P226" s="4"/>
     </row>
-    <row r="227" spans="2:16" ht="15.75">
+    <row r="227" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="P227" s="4"/>
     </row>
-    <row r="228" spans="2:16" ht="15.75">
+    <row r="228" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="P228" s="4"/>
     </row>
-    <row r="229" spans="2:16" ht="15.75">
+    <row r="229" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="P229" s="4"/>
     </row>
-    <row r="230" spans="2:16" ht="15.75">
+    <row r="230" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="P230" s="4"/>
     </row>
-    <row r="231" spans="2:16" ht="15.75">
+    <row r="231" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="P231" s="4"/>
     </row>
-    <row r="232" spans="2:16" ht="15.75">
+    <row r="232" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="P232" s="4"/>
     </row>
-    <row r="233" spans="2:16" ht="15.75">
+    <row r="233" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="P233" s="4"/>
     </row>
-    <row r="234" spans="2:16" ht="15.75">
+    <row r="234" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="P234" s="4"/>
     </row>
-    <row r="235" spans="2:16" ht="15.75">
+    <row r="235" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="P235" s="4"/>
     </row>
-    <row r="236" spans="2:16" ht="15.75">
+    <row r="236" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="P236" s="4"/>
     </row>
-    <row r="237" spans="2:16" ht="15.75">
+    <row r="237" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="P237" s="4"/>
     </row>
-    <row r="238" spans="2:16" ht="15.75">
+    <row r="238" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="P238" s="4"/>
     </row>
-    <row r="239" spans="2:16" ht="15.75">
+    <row r="239" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="P239" s="4"/>
     </row>
-    <row r="240" spans="2:16" ht="15.75">
+    <row r="240" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="P240" s="4"/>
     </row>
-    <row r="241" spans="2:16" ht="15.75">
+    <row r="241" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="P241" s="4"/>
     </row>
-    <row r="242" spans="2:16" ht="15.75">
+    <row r="242" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="P242" s="4"/>
     </row>
-    <row r="243" spans="2:16" ht="15.75">
+    <row r="243" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="2:16" ht="15.75">
+    <row r="244" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="2:16" ht="15.75">
+    <row r="245" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="2:16" ht="15.75">
+    <row r="246" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="2:16" ht="15.75">
+    <row r="247" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="2:16" ht="15.75">
+    <row r="248" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="2:16" ht="15.75">
+    <row r="249" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="2:16" ht="15.75">
+    <row r="250" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="2:16" ht="15.75">
+    <row r="251" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="2:16" ht="15.75">
+    <row r="252" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="2:16" ht="15.75">
+    <row r="253" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="2:16" ht="15.75">
+    <row r="254" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="2:16" ht="15.75">
+    <row r="255" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="2:16" ht="15.75">
+    <row r="256" spans="2:16" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="2:4" ht="15.75">
+    <row r="257" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="2:4" ht="15.75">
+    <row r="258" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="2:4" ht="15.75">
+    <row r="259" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="2:4" ht="15.75">
+    <row r="260" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="2:4" ht="15.75">
+    <row r="261" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="2:4" ht="15.75">
+    <row r="262" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="2:4" ht="15.75">
+    <row r="263" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="2:4" ht="15.75">
+    <row r="264" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="2:4" ht="15.75">
+    <row r="265" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="2:4" ht="15.75">
+    <row r="266" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="2:4" ht="15.75">
+    <row r="267" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="2:4" ht="15.75">
+    <row r="268" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="2:4" ht="15.75">
+    <row r="269" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="2:4" ht="15.75">
+    <row r="270" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="2:4" ht="15.75">
+    <row r="271" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="2:4" ht="15.75">
+    <row r="272" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="2:4" ht="15.75">
+    <row r="273" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="2:4" ht="15.75">
+    <row r="274" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="2:4" ht="15.75">
+    <row r="275" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="2:4" ht="15.75">
+    <row r="276" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="2:4" ht="15.75">
+    <row r="277" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="2:4" ht="15.75">
+    <row r="278" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="2:4" ht="15.75">
+    <row r="279" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="2:4" ht="15.75">
+    <row r="280" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="2:4" ht="15.75">
+    <row r="281" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="2:4" ht="15.75">
+    <row r="282" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="2:4" ht="15.75">
+    <row r="283" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="2:4" ht="15.75">
+    <row r="284" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="2:4" ht="15.75">
+    <row r="285" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="2:4" ht="15.75">
+    <row r="286" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="2:4" ht="15.75">
+    <row r="287" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="2:4" ht="15.75">
+    <row r="288" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="2:4" ht="15.75">
+    <row r="289" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="2:4" ht="15.75">
+    <row r="290" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="2:4" ht="15.75">
+    <row r="291" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="2:4" ht="15.75">
+    <row r="292" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="2:4" ht="15.75">
+    <row r="293" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="2:4" ht="15.75">
+    <row r="294" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="2:4" ht="15.75">
+    <row r="295" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="2:4" ht="15.75">
+    <row r="296" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="2:4" ht="15.75">
+    <row r="297" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="2:4" ht="15.75">
+    <row r="298" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="2:4" ht="15.75">
+    <row r="299" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="2:4" ht="15.75">
+    <row r="300" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="2:4" ht="15.75">
+    <row r="301" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="2:4" ht="15.75">
+    <row r="302" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="2:4" ht="15.75">
+    <row r="303" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="2:4" ht="15.75">
+    <row r="304" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="2:4" ht="15.75">
+    <row r="305" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="2:4" ht="15.75">
+    <row r="306" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="2:4" ht="15.75">
+    <row r="307" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="2:4" ht="15.75">
+    <row r="308" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="2:4" ht="15.75">
+    <row r="309" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="2:4" ht="15.75">
+    <row r="310" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="2:4" ht="15.75">
+    <row r="311" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="2:4" ht="15.75">
+    <row r="312" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="2:4" ht="15.75">
+    <row r="313" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="2:4" ht="15.75">
+    <row r="314" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="2:4" ht="15.75">
+    <row r="315" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="2:4" ht="15.75">
+    <row r="316" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="2:4" ht="15.75">
+    <row r="317" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="2:4" ht="15.75">
+    <row r="318" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="2:4" ht="15.75">
+    <row r="319" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="2:4" ht="15.75">
+    <row r="320" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="2:4" ht="15.75">
+    <row r="321" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="2:4" ht="15.75">
+    <row r="322" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="2:4" ht="15.75">
+    <row r="323" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="2:4" ht="15.75">
+    <row r="324" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="2:4" ht="15.75">
+    <row r="325" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="2:4" ht="15.75">
+    <row r="326" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="2:4" ht="15.75">
+    <row r="327" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="2:4" ht="15.75">
+    <row r="328" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="2:4" ht="15.75">
+    <row r="329" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="2:4" ht="15.75">
+    <row r="330" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="2:4" ht="15.75">
+    <row r="331" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="2:4" ht="15.75">
+    <row r="332" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="2:4" ht="15.75">
+    <row r="333" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="2:4" ht="15.75">
+    <row r="334" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="2:4" ht="15.75">
+    <row r="335" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="2:4" ht="15.75">
+    <row r="336" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="2:4" ht="15.75">
+    <row r="337" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="2:4" ht="15.75">
+    <row r="338" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="2:4" ht="15.75">
+    <row r="339" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="2:4" ht="15.75">
+    <row r="340" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="2:4" ht="15.75">
+    <row r="341" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="2:4" ht="15.75">
+    <row r="342" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="2:4" ht="15.75">
+    <row r="343" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="2:4" ht="15.75">
+    <row r="344" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="2:4" ht="15.75">
+    <row r="345" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="2:4" ht="15.75">
+    <row r="346" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="2:4" ht="15.75">
+    <row r="347" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="2:4" ht="15.75">
+    <row r="348" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="2:4" ht="15.75">
+    <row r="349" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="2:4" ht="15.75">
+    <row r="350" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="2:4" ht="15.75">
+    <row r="351" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="2:4" ht="15.75">
+    <row r="352" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="2:4" ht="15.75">
+    <row r="353" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="2:4" ht="15.75">
+    <row r="354" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="2:4" ht="15.75">
+    <row r="355" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="2:4" ht="15.75">
+    <row r="356" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="2:4" ht="15.75">
+    <row r="357" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="2:4" ht="15.75">
+    <row r="358" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="2:4" ht="15.75">
+    <row r="359" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="2:4" ht="15.75">
+    <row r="360" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="2:4" ht="15.75">
+    <row r="361" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="2:4" ht="15.75">
+    <row r="362" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="2:4" ht="15.75">
+    <row r="363" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="2:4" ht="15.75">
+    <row r="364" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="2:4" ht="15.75">
+    <row r="365" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="2:4" ht="15.75">
+    <row r="366" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="2:4" ht="15.75">
+    <row r="367" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="2:4" ht="15.75">
+    <row r="368" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="2:4" ht="15.75">
+    <row r="369" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="2:4" ht="15.75">
+    <row r="370" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="2:4" ht="15.75">
+    <row r="371" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="2:4" ht="15.75">
+    <row r="372" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="2:4" ht="15.75">
+    <row r="373" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="2:4" ht="15.75">
+    <row r="374" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="2:4" ht="15.75">
+    <row r="375" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="2:4" ht="15.75">
+    <row r="376" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="2:4" ht="15.75">
+    <row r="377" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="2:4" ht="15.75">
+    <row r="378" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="2:4" ht="15.75">
+    <row r="379" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="2:4" ht="15.75">
+    <row r="380" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="2:4" ht="15.75">
+    <row r="381" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="2:4" ht="15.75">
+    <row r="382" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="2:4" ht="15.75">
+    <row r="383" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="2:4" ht="15.75">
+    <row r="384" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="2:4" ht="15.75">
+    <row r="385" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="2:4" ht="15.75">
+    <row r="386" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="2:4" ht="15.75">
+    <row r="387" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="2:4" ht="15.75">
+    <row r="388" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="2:4" ht="15.75">
+    <row r="389" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="2:4" ht="15.75">
+    <row r="390" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="2:4" ht="15.75">
+    <row r="391" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="2:4" ht="15.75">
+    <row r="392" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="2:4" ht="15.75">
+    <row r="393" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="2:4" ht="15.75">
+    <row r="394" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="2:4" ht="15.75">
+    <row r="395" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="2:4" ht="15.75">
+    <row r="396" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="2:4" ht="15.75">
+    <row r="397" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="2:4" ht="15.75">
+    <row r="398" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="2:4" ht="15.75">
+    <row r="399" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="2:4" ht="15.75">
+    <row r="400" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="2:4" ht="15.75">
+    <row r="401" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="2:4" ht="15.75">
+    <row r="402" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="2:4" ht="15.75">
+    <row r="403" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="2:4" ht="15.75">
+    <row r="404" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B404" s="2"/>
       <c r="C404" s="2"/>
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="2:4" ht="15.75">
+    <row r="405" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B405" s="2"/>
       <c r="C405" s="2"/>
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="2:4" ht="15.75">
+    <row r="406" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B406" s="2"/>
       <c r="C406" s="2"/>
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="2:4" ht="15.75">
+    <row r="407" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B407" s="2"/>
       <c r="C407" s="2"/>
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="2:4" ht="15.75">
+    <row r="408" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B408" s="2"/>
       <c r="C408" s="2"/>
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="2:4" ht="15.75">
+    <row r="409" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="2:4" ht="15.75">
+    <row r="410" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B410" s="2"/>
       <c r="C410" s="2"/>
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="2:4" ht="15.75">
+    <row r="411" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B411" s="2"/>
       <c r="C411" s="2"/>
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="2:4" ht="15.75">
+    <row r="412" spans="2:4" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
       <c r="D412" s="2"/>

</xml_diff>